<commit_message>
init turns and load the next one.
</commit_message>
<xml_diff>
--- a/docs/formule.xlsx
+++ b/docs/formule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a\projects\vitalegi\rpg-adventure\jarg-fe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a\projects\vitalegi\rpg-adventure\jarg-fe\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285F5884-D935-4166-88A7-1E143634AACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFDB5D5-F27F-4460-B5E5-124EBD5034D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="25870" windowHeight="14050" activeTab="2" xr2:uid="{B81DC7DF-F854-4748-8482-B1A1A73A8B46}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="25870" windowHeight="14050" xr2:uid="{B81DC7DF-F854-4748-8482-B1A1A73A8B46}"/>
   </bookViews>
   <sheets>
     <sheet name="turn speed" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
   <si>
     <t>target</t>
   </si>
@@ -184,15 +184,97 @@
   </si>
   <si>
     <t>increase ratio</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>bonus</t>
+  </si>
+  <si>
+    <t>speed*</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>ticks #1</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>action effect</t>
+  </si>
+  <si>
+    <t>max ticks ratio</t>
+  </si>
+  <si>
+    <t>ticks #2</t>
+  </si>
+  <si>
+    <t>SUM*</t>
+  </si>
+  <si>
+    <t>base ticks</t>
+  </si>
+  <si>
+    <t>ticks</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>agi</t>
+  </si>
+  <si>
+    <t>ICV min</t>
+  </si>
+  <si>
+    <t>ICV max</t>
+  </si>
+  <si>
+    <t>AGI min</t>
+  </si>
+  <si>
+    <t>AGI max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -254,7 +336,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -264,6 +346,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -580,15 +663,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4657505-48FE-4560-82C2-C056CEDDC0B2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:X96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -598,8 +686,29 @@
       <c r="C1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -609,8 +718,36 @@
       <c r="C2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>1.5</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <f>H2*I2*J2</f>
+        <v>300</v>
+      </c>
+      <c r="L2" s="9">
+        <f>(K$12/H2)</f>
+        <v>6</v>
+      </c>
+      <c r="M2" s="9">
+        <f>MIN(MIN($L$2:$L$11)*$K$15,L2)/(I2*J2)+$K$16</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="8">
+        <f>ROUNDUP(M2,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -620,8 +757,36 @@
       <c r="C3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K7" si="0">H3*I3*J3</f>
+        <v>200</v>
+      </c>
+      <c r="L3" s="9">
+        <f t="shared" ref="L3:L7" si="1">(K$12/H3)</f>
+        <v>6</v>
+      </c>
+      <c r="M3" s="9">
+        <f>MIN(MIN($L$2:$L$11)*$K$15,L3)/(I3*J3)+$K$16</f>
+        <v>1.5</v>
+      </c>
+      <c r="N3" s="8">
+        <f t="shared" ref="N3:N7" si="2">ROUNDUP(M3,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -632,6 +797,1906 @@
       <c r="C4">
         <f>(C1-C2)/C3</f>
         <v>99</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="L4" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M4" s="9">
+        <f t="shared" ref="M4:M7" si="3">MIN(MIN($L$2:$L$11)*$K$15,L4)/(I4*J4)+$K$16</f>
+        <v>6</v>
+      </c>
+      <c r="N4" s="8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5">
+        <v>50</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="L5" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="L6" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N6" s="8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="L7" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M7" s="9">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N7" s="8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12">
+        <f>SUM(H2:H7)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13">
+        <f>SUM(K2:K10)</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14">
+        <f>AVERAGE(K2:K10)</f>
+        <v>116.66666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" t="s">
+        <v>71</v>
+      </c>
+      <c r="J19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <f>ROUND(H20/MAX(H$20:H$28)*255,0)</f>
+        <v>85</v>
+      </c>
+      <c r="P20" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>75</v>
+      </c>
+      <c r="R20" t="s">
+        <v>70</v>
+      </c>
+      <c r="T20" t="s">
+        <v>74</v>
+      </c>
+      <c r="U20" t="s">
+        <v>75</v>
+      </c>
+      <c r="V20" t="s">
+        <v>72</v>
+      </c>
+      <c r="W20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21">
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21:I28" si="4">ROUND(H21/MAX(H$20:H$28)*255,0)</f>
+        <v>68</v>
+      </c>
+      <c r="O21" t="str">
+        <f>_xlfn.CONCAT("{""ge"": ",P21,", ""le"": ",Q21,", ""ts"": ",R21,"},")</f>
+        <v>{"ge": 0, "le": 0, "ts": 28},</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>28</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>83</v>
+      </c>
+      <c r="W21">
+        <v>84</v>
+      </c>
+      <c r="X21" t="str">
+        <f>_xlfn.CONCAT("{""ge"": ",T21,", ""le"": ",U21,", ""icv_min"": ",V21,", ""icv_max"": ",W21,"},")</f>
+        <v>{"ge": 0, "le": 1, "icv_min": 83, "icv_max": 84},</v>
+      </c>
+    </row>
+    <row r="22" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" ref="O22:O39" si="5">_xlfn.CONCAT("{""ge"": ",P22,", ""le"": ",Q22,", ""ts"": ",R22,"},")</f>
+        <v>{"ge": 1, "le": 1, "ts": 26},</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>26</v>
+      </c>
+      <c r="T22">
+        <v>2</v>
+      </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
+      <c r="V22">
+        <v>77</v>
+      </c>
+      <c r="W22">
+        <v>78</v>
+      </c>
+      <c r="X22" t="str">
+        <f t="shared" ref="X22:X85" si="6">_xlfn.CONCAT("{""ge"": ",T22,", ""le"": ",U22,", ""icv_min"": ",V22,", ""icv_max"": ",W22,"},")</f>
+        <v>{"ge": 2, "le": 2, "icv_min": 77, "icv_max": 78},</v>
+      </c>
+    </row>
+    <row r="23" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23">
+        <v>9</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 2, "le": 2, "ts": 24},</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>2</v>
+      </c>
+      <c r="R23">
+        <v>24</v>
+      </c>
+      <c r="T23">
+        <v>3</v>
+      </c>
+      <c r="U23">
+        <v>3</v>
+      </c>
+      <c r="V23">
+        <v>71</v>
+      </c>
+      <c r="W23">
+        <v>72</v>
+      </c>
+      <c r="X23" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 3, "le": 3, "icv_min": 71, "icv_max": 72},</v>
+      </c>
+    </row>
+    <row r="24" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 3, "le": 3, "ts": 22},</v>
+      </c>
+      <c r="P24">
+        <v>3</v>
+      </c>
+      <c r="Q24">
+        <v>3</v>
+      </c>
+      <c r="R24">
+        <v>22</v>
+      </c>
+      <c r="T24">
+        <v>4</v>
+      </c>
+      <c r="U24">
+        <v>4</v>
+      </c>
+      <c r="V24">
+        <v>59</v>
+      </c>
+      <c r="W24">
+        <v>60</v>
+      </c>
+      <c r="X24" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 4, "le": 4, "icv_min": 59, "icv_max": 60},</v>
+      </c>
+    </row>
+    <row r="25" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 4, "le": 4, "ts": 20},</v>
+      </c>
+      <c r="P25">
+        <v>4</v>
+      </c>
+      <c r="Q25">
+        <v>4</v>
+      </c>
+      <c r="R25">
+        <v>20</v>
+      </c>
+      <c r="T25">
+        <v>5</v>
+      </c>
+      <c r="U25">
+        <v>5</v>
+      </c>
+      <c r="V25">
+        <v>47</v>
+      </c>
+      <c r="W25">
+        <v>48</v>
+      </c>
+      <c r="X25" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 5, "le": 5, "icv_min": 47, "icv_max": 48},</v>
+      </c>
+    </row>
+    <row r="26" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26">
+        <v>20</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>170</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 5, "le": 6, "ts": 16},</v>
+      </c>
+      <c r="P26">
+        <v>5</v>
+      </c>
+      <c r="Q26">
+        <v>6</v>
+      </c>
+      <c r="R26">
+        <v>16</v>
+      </c>
+      <c r="T26">
+        <v>6</v>
+      </c>
+      <c r="U26">
+        <v>6</v>
+      </c>
+      <c r="V26">
+        <v>46</v>
+      </c>
+      <c r="W26">
+        <v>48</v>
+      </c>
+      <c r="X26" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 6, "le": 6, "icv_min": 46, "icv_max": 48},</v>
+      </c>
+    </row>
+    <row r="27" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27">
+        <v>12</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
+        <v>102</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 7, "le": 9, "ts": 15},</v>
+      </c>
+      <c r="P27">
+        <v>7</v>
+      </c>
+      <c r="Q27">
+        <v>9</v>
+      </c>
+      <c r="R27">
+        <v>15</v>
+      </c>
+      <c r="T27">
+        <v>7</v>
+      </c>
+      <c r="U27">
+        <v>7</v>
+      </c>
+      <c r="V27">
+        <v>44</v>
+      </c>
+      <c r="W27">
+        <v>45</v>
+      </c>
+      <c r="X27" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 7, "le": 7, "icv_min": 44, "icv_max": 45},</v>
+      </c>
+    </row>
+    <row r="28" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28">
+        <v>30</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 10, "le": 11, "ts": 14},</v>
+      </c>
+      <c r="P28">
+        <v>10</v>
+      </c>
+      <c r="Q28">
+        <v>11</v>
+      </c>
+      <c r="R28">
+        <v>14</v>
+      </c>
+      <c r="T28">
+        <v>8</v>
+      </c>
+      <c r="U28">
+        <v>8</v>
+      </c>
+      <c r="V28">
+        <v>43</v>
+      </c>
+      <c r="W28">
+        <v>45</v>
+      </c>
+      <c r="X28" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 8, "le": 8, "icv_min": 43, "icv_max": 45},</v>
+      </c>
+    </row>
+    <row r="29" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="O29" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 12, "le": 14, "ts": 13},</v>
+      </c>
+      <c r="P29">
+        <v>12</v>
+      </c>
+      <c r="Q29">
+        <v>14</v>
+      </c>
+      <c r="R29">
+        <v>13</v>
+      </c>
+      <c r="T29">
+        <v>9</v>
+      </c>
+      <c r="U29">
+        <v>9</v>
+      </c>
+      <c r="V29">
+        <v>42</v>
+      </c>
+      <c r="W29">
+        <v>45</v>
+      </c>
+      <c r="X29" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 9, "le": 9, "icv_min": 42, "icv_max": 45},</v>
+      </c>
+    </row>
+    <row r="30" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="O30" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 15, "le": 16, "ts": 12},</v>
+      </c>
+      <c r="P30">
+        <v>15</v>
+      </c>
+      <c r="Q30">
+        <v>16</v>
+      </c>
+      <c r="R30">
+        <v>12</v>
+      </c>
+      <c r="T30">
+        <v>10</v>
+      </c>
+      <c r="U30">
+        <v>10</v>
+      </c>
+      <c r="V30">
+        <v>41</v>
+      </c>
+      <c r="W30">
+        <v>42</v>
+      </c>
+      <c r="X30" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 10, "le": 10, "icv_min": 41, "icv_max": 42},</v>
+      </c>
+    </row>
+    <row r="31" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="O31" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 17, "le": 18, "ts": 11},</v>
+      </c>
+      <c r="P31">
+        <v>17</v>
+      </c>
+      <c r="Q31">
+        <v>18</v>
+      </c>
+      <c r="R31">
+        <v>11</v>
+      </c>
+      <c r="T31">
+        <v>11</v>
+      </c>
+      <c r="U31">
+        <v>11</v>
+      </c>
+      <c r="V31">
+        <v>40</v>
+      </c>
+      <c r="W31">
+        <v>42</v>
+      </c>
+      <c r="X31" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 11, "le": 11, "icv_min": 40, "icv_max": 42},</v>
+      </c>
+    </row>
+    <row r="32" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="O32" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 19, "le": 22, "ts": 10},</v>
+      </c>
+      <c r="P32">
+        <v>19</v>
+      </c>
+      <c r="Q32">
+        <v>22</v>
+      </c>
+      <c r="R32">
+        <v>10</v>
+      </c>
+      <c r="T32">
+        <v>12</v>
+      </c>
+      <c r="U32">
+        <v>12</v>
+      </c>
+      <c r="V32">
+        <v>38</v>
+      </c>
+      <c r="W32">
+        <v>39</v>
+      </c>
+      <c r="X32" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 12, "le": 12, "icv_min": 38, "icv_max": 39},</v>
+      </c>
+    </row>
+    <row r="33" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O33" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 23, "le": 28, "ts": 9},</v>
+      </c>
+      <c r="P33">
+        <v>23</v>
+      </c>
+      <c r="Q33">
+        <v>28</v>
+      </c>
+      <c r="R33">
+        <v>9</v>
+      </c>
+      <c r="T33">
+        <v>13</v>
+      </c>
+      <c r="U33">
+        <v>13</v>
+      </c>
+      <c r="V33">
+        <v>37</v>
+      </c>
+      <c r="W33">
+        <v>39</v>
+      </c>
+      <c r="X33" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 13, "le": 13, "icv_min": 37, "icv_max": 39},</v>
+      </c>
+    </row>
+    <row r="34" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O34" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 29, "le": 34, "ts": 8},</v>
+      </c>
+      <c r="P34">
+        <v>29</v>
+      </c>
+      <c r="Q34">
+        <v>34</v>
+      </c>
+      <c r="R34">
+        <v>8</v>
+      </c>
+      <c r="T34">
+        <v>14</v>
+      </c>
+      <c r="U34">
+        <v>14</v>
+      </c>
+      <c r="V34">
+        <v>36</v>
+      </c>
+      <c r="W34">
+        <v>39</v>
+      </c>
+      <c r="X34" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 14, "le": 14, "icv_min": 36, "icv_max": 39},</v>
+      </c>
+    </row>
+    <row r="35" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O35" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 35, "le": 43, "ts": 7},</v>
+      </c>
+      <c r="P35">
+        <v>35</v>
+      </c>
+      <c r="Q35">
+        <v>43</v>
+      </c>
+      <c r="R35">
+        <v>7</v>
+      </c>
+      <c r="T35">
+        <v>15</v>
+      </c>
+      <c r="U35">
+        <v>15</v>
+      </c>
+      <c r="V35">
+        <v>35</v>
+      </c>
+      <c r="W35">
+        <v>36</v>
+      </c>
+      <c r="X35" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 15, "le": 15, "icv_min": 35, "icv_max": 36},</v>
+      </c>
+    </row>
+    <row r="36" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O36" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 44, "le": 61, "ts": 6},</v>
+      </c>
+      <c r="P36">
+        <v>44</v>
+      </c>
+      <c r="Q36">
+        <v>61</v>
+      </c>
+      <c r="R36">
+        <v>6</v>
+      </c>
+      <c r="T36">
+        <v>16</v>
+      </c>
+      <c r="U36">
+        <v>16</v>
+      </c>
+      <c r="V36">
+        <v>34</v>
+      </c>
+      <c r="W36">
+        <v>36</v>
+      </c>
+      <c r="X36" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 16, "le": 16, "icv_min": 34, "icv_max": 36},</v>
+      </c>
+    </row>
+    <row r="37" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O37" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 62, "le": 97, "ts": 5},</v>
+      </c>
+      <c r="P37">
+        <v>62</v>
+      </c>
+      <c r="Q37">
+        <v>97</v>
+      </c>
+      <c r="R37">
+        <v>5</v>
+      </c>
+      <c r="T37">
+        <v>17</v>
+      </c>
+      <c r="U37">
+        <v>17</v>
+      </c>
+      <c r="V37">
+        <v>32</v>
+      </c>
+      <c r="W37">
+        <v>33</v>
+      </c>
+      <c r="X37" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 17, "le": 17, "icv_min": 32, "icv_max": 33},</v>
+      </c>
+    </row>
+    <row r="38" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O38" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 98, "le": 169, "ts": 4},</v>
+      </c>
+      <c r="P38">
+        <v>98</v>
+      </c>
+      <c r="Q38">
+        <v>169</v>
+      </c>
+      <c r="R38">
+        <v>4</v>
+      </c>
+      <c r="T38">
+        <v>18</v>
+      </c>
+      <c r="U38">
+        <v>18</v>
+      </c>
+      <c r="V38">
+        <v>31</v>
+      </c>
+      <c r="W38">
+        <v>33</v>
+      </c>
+      <c r="X38" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 18, "le": 18, "icv_min": 31, "icv_max": 33},</v>
+      </c>
+    </row>
+    <row r="39" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O39" t="str">
+        <f t="shared" si="5"/>
+        <v>{"ge": 170, "le": 255, "ts": 3},</v>
+      </c>
+      <c r="P39">
+        <v>170</v>
+      </c>
+      <c r="Q39">
+        <v>255</v>
+      </c>
+      <c r="R39">
+        <v>3</v>
+      </c>
+      <c r="T39">
+        <v>19</v>
+      </c>
+      <c r="U39">
+        <v>19</v>
+      </c>
+      <c r="V39">
+        <v>29</v>
+      </c>
+      <c r="W39">
+        <v>30</v>
+      </c>
+      <c r="X39" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 19, "le": 19, "icv_min": 29, "icv_max": 30},</v>
+      </c>
+    </row>
+    <row r="40" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="T40">
+        <v>20</v>
+      </c>
+      <c r="U40">
+        <v>20</v>
+      </c>
+      <c r="V40">
+        <v>28</v>
+      </c>
+      <c r="W40">
+        <v>30</v>
+      </c>
+      <c r="X40" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 20, "le": 20, "icv_min": 28, "icv_max": 30},</v>
+      </c>
+    </row>
+    <row r="41" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="T41">
+        <v>21</v>
+      </c>
+      <c r="U41">
+        <v>21</v>
+      </c>
+      <c r="V41">
+        <v>27</v>
+      </c>
+      <c r="W41">
+        <v>30</v>
+      </c>
+      <c r="X41" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 21, "le": 21, "icv_min": 27, "icv_max": 30},</v>
+      </c>
+    </row>
+    <row r="42" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="T42">
+        <v>22</v>
+      </c>
+      <c r="U42">
+        <v>22</v>
+      </c>
+      <c r="V42">
+        <v>26</v>
+      </c>
+      <c r="W42">
+        <v>30</v>
+      </c>
+      <c r="X42" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 22, "le": 22, "icv_min": 26, "icv_max": 30},</v>
+      </c>
+    </row>
+    <row r="43" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="T43">
+        <v>23</v>
+      </c>
+      <c r="U43">
+        <v>23</v>
+      </c>
+      <c r="V43">
+        <v>26</v>
+      </c>
+      <c r="W43">
+        <v>27</v>
+      </c>
+      <c r="X43" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 23, "le": 23, "icv_min": 26, "icv_max": 27},</v>
+      </c>
+    </row>
+    <row r="44" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="T44">
+        <v>24</v>
+      </c>
+      <c r="U44">
+        <v>24</v>
+      </c>
+      <c r="V44">
+        <v>25</v>
+      </c>
+      <c r="W44">
+        <v>27</v>
+      </c>
+      <c r="X44" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 24, "le": 24, "icv_min": 25, "icv_max": 27},</v>
+      </c>
+    </row>
+    <row r="45" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="T45">
+        <v>25</v>
+      </c>
+      <c r="U45">
+        <v>25</v>
+      </c>
+      <c r="V45">
+        <v>24</v>
+      </c>
+      <c r="W45">
+        <v>27</v>
+      </c>
+      <c r="X45" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 25, "le": 25, "icv_min": 24, "icv_max": 27},</v>
+      </c>
+    </row>
+    <row r="46" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="T46">
+        <v>26</v>
+      </c>
+      <c r="U46">
+        <v>26</v>
+      </c>
+      <c r="V46">
+        <v>23</v>
+      </c>
+      <c r="W46">
+        <v>27</v>
+      </c>
+      <c r="X46" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 26, "le": 26, "icv_min": 23, "icv_max": 27},</v>
+      </c>
+    </row>
+    <row r="47" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="T47">
+        <v>27</v>
+      </c>
+      <c r="U47">
+        <v>27</v>
+      </c>
+      <c r="V47">
+        <v>22</v>
+      </c>
+      <c r="W47">
+        <v>27</v>
+      </c>
+      <c r="X47" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 27, "le": 27, "icv_min": 22, "icv_max": 27},</v>
+      </c>
+    </row>
+    <row r="48" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="T48">
+        <v>28</v>
+      </c>
+      <c r="U48">
+        <v>28</v>
+      </c>
+      <c r="V48">
+        <v>21</v>
+      </c>
+      <c r="W48">
+        <v>27</v>
+      </c>
+      <c r="X48" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 28, "le": 28, "icv_min": 21, "icv_max": 27},</v>
+      </c>
+    </row>
+    <row r="49" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T49">
+        <v>29</v>
+      </c>
+      <c r="U49">
+        <v>29</v>
+      </c>
+      <c r="V49">
+        <v>23</v>
+      </c>
+      <c r="W49">
+        <v>24</v>
+      </c>
+      <c r="X49" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 29, "le": 29, "icv_min": 23, "icv_max": 24},</v>
+      </c>
+    </row>
+    <row r="50" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T50">
+        <v>30</v>
+      </c>
+      <c r="U50">
+        <v>30</v>
+      </c>
+      <c r="V50">
+        <v>22</v>
+      </c>
+      <c r="W50">
+        <v>24</v>
+      </c>
+      <c r="X50" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 30, "le": 30, "icv_min": 22, "icv_max": 24},</v>
+      </c>
+    </row>
+    <row r="51" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T51">
+        <v>31</v>
+      </c>
+      <c r="U51">
+        <v>31</v>
+      </c>
+      <c r="V51">
+        <v>21</v>
+      </c>
+      <c r="W51">
+        <v>24</v>
+      </c>
+      <c r="X51" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 31, "le": 31, "icv_min": 21, "icv_max": 24},</v>
+      </c>
+    </row>
+    <row r="52" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T52">
+        <v>32</v>
+      </c>
+      <c r="U52">
+        <v>32</v>
+      </c>
+      <c r="V52">
+        <v>20</v>
+      </c>
+      <c r="W52">
+        <v>24</v>
+      </c>
+      <c r="X52" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 32, "le": 32, "icv_min": 20, "icv_max": 24},</v>
+      </c>
+    </row>
+    <row r="53" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T53">
+        <v>33</v>
+      </c>
+      <c r="U53">
+        <v>33</v>
+      </c>
+      <c r="V53">
+        <v>19</v>
+      </c>
+      <c r="W53">
+        <v>24</v>
+      </c>
+      <c r="X53" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 33, "le": 33, "icv_min": 19, "icv_max": 24},</v>
+      </c>
+    </row>
+    <row r="54" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T54">
+        <v>34</v>
+      </c>
+      <c r="U54">
+        <v>34</v>
+      </c>
+      <c r="V54">
+        <v>18</v>
+      </c>
+      <c r="W54">
+        <v>24</v>
+      </c>
+      <c r="X54" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 34, "le": 34, "icv_min": 18, "icv_max": 24},</v>
+      </c>
+    </row>
+    <row r="55" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T55">
+        <v>35</v>
+      </c>
+      <c r="U55">
+        <v>35</v>
+      </c>
+      <c r="V55">
+        <v>20</v>
+      </c>
+      <c r="W55">
+        <v>21</v>
+      </c>
+      <c r="X55" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 35, "le": 35, "icv_min": 20, "icv_max": 21},</v>
+      </c>
+    </row>
+    <row r="56" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T56">
+        <v>36</v>
+      </c>
+      <c r="U56">
+        <v>36</v>
+      </c>
+      <c r="V56">
+        <v>19</v>
+      </c>
+      <c r="W56">
+        <v>21</v>
+      </c>
+      <c r="X56" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 36, "le": 36, "icv_min": 19, "icv_max": 21},</v>
+      </c>
+    </row>
+    <row r="57" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T57">
+        <v>37</v>
+      </c>
+      <c r="U57">
+        <v>37</v>
+      </c>
+      <c r="V57">
+        <v>18</v>
+      </c>
+      <c r="W57">
+        <v>21</v>
+      </c>
+      <c r="X57" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 37, "le": 37, "icv_min": 18, "icv_max": 21},</v>
+      </c>
+    </row>
+    <row r="58" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T58">
+        <v>38</v>
+      </c>
+      <c r="U58">
+        <v>38</v>
+      </c>
+      <c r="V58">
+        <v>17</v>
+      </c>
+      <c r="W58">
+        <v>21</v>
+      </c>
+      <c r="X58" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 38, "le": 38, "icv_min": 17, "icv_max": 21},</v>
+      </c>
+    </row>
+    <row r="59" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T59">
+        <v>39</v>
+      </c>
+      <c r="U59">
+        <v>39</v>
+      </c>
+      <c r="V59">
+        <v>16</v>
+      </c>
+      <c r="W59">
+        <v>21</v>
+      </c>
+      <c r="X59" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 39, "le": 39, "icv_min": 16, "icv_max": 21},</v>
+      </c>
+    </row>
+    <row r="60" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T60">
+        <v>40</v>
+      </c>
+      <c r="U60">
+        <v>40</v>
+      </c>
+      <c r="V60">
+        <v>15</v>
+      </c>
+      <c r="W60">
+        <v>21</v>
+      </c>
+      <c r="X60" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 40, "le": 40, "icv_min": 15, "icv_max": 21},</v>
+      </c>
+    </row>
+    <row r="61" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T61">
+        <v>41</v>
+      </c>
+      <c r="U61">
+        <v>41</v>
+      </c>
+      <c r="V61">
+        <v>14</v>
+      </c>
+      <c r="W61">
+        <v>21</v>
+      </c>
+      <c r="X61" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 41, "le": 41, "icv_min": 14, "icv_max": 21},</v>
+      </c>
+    </row>
+    <row r="62" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T62">
+        <v>42</v>
+      </c>
+      <c r="U62">
+        <v>42</v>
+      </c>
+      <c r="V62">
+        <v>13</v>
+      </c>
+      <c r="W62">
+        <v>21</v>
+      </c>
+      <c r="X62" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 42, "le": 42, "icv_min": 13, "icv_max": 21},</v>
+      </c>
+    </row>
+    <row r="63" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T63">
+        <v>43</v>
+      </c>
+      <c r="U63">
+        <v>43</v>
+      </c>
+      <c r="V63">
+        <v>12</v>
+      </c>
+      <c r="W63">
+        <v>21</v>
+      </c>
+      <c r="X63" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 43, "le": 43, "icv_min": 12, "icv_max": 21},</v>
+      </c>
+    </row>
+    <row r="64" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T64">
+        <v>44</v>
+      </c>
+      <c r="U64">
+        <v>45</v>
+      </c>
+      <c r="V64">
+        <v>17</v>
+      </c>
+      <c r="W64">
+        <v>18</v>
+      </c>
+      <c r="X64" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 44, "le": 45, "icv_min": 17, "icv_max": 18},</v>
+      </c>
+    </row>
+    <row r="65" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T65">
+        <v>46</v>
+      </c>
+      <c r="U65">
+        <v>47</v>
+      </c>
+      <c r="V65">
+        <v>16</v>
+      </c>
+      <c r="W65">
+        <v>18</v>
+      </c>
+      <c r="X65" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 46, "le": 47, "icv_min": 16, "icv_max": 18},</v>
+      </c>
+    </row>
+    <row r="66" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T66">
+        <v>48</v>
+      </c>
+      <c r="U66">
+        <v>49</v>
+      </c>
+      <c r="V66">
+        <v>15</v>
+      </c>
+      <c r="W66">
+        <v>18</v>
+      </c>
+      <c r="X66" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 48, "le": 49, "icv_min": 15, "icv_max": 18},</v>
+      </c>
+    </row>
+    <row r="67" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T67">
+        <v>50</v>
+      </c>
+      <c r="U67">
+        <v>51</v>
+      </c>
+      <c r="V67">
+        <v>14</v>
+      </c>
+      <c r="W67">
+        <v>18</v>
+      </c>
+      <c r="X67" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 50, "le": 51, "icv_min": 14, "icv_max": 18},</v>
+      </c>
+    </row>
+    <row r="68" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T68">
+        <v>52</v>
+      </c>
+      <c r="U68">
+        <v>53</v>
+      </c>
+      <c r="V68">
+        <v>13</v>
+      </c>
+      <c r="W68">
+        <v>18</v>
+      </c>
+      <c r="X68" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 52, "le": 53, "icv_min": 13, "icv_max": 18},</v>
+      </c>
+    </row>
+    <row r="69" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T69">
+        <v>54</v>
+      </c>
+      <c r="U69">
+        <v>55</v>
+      </c>
+      <c r="V69">
+        <v>12</v>
+      </c>
+      <c r="W69">
+        <v>18</v>
+      </c>
+      <c r="X69" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 54, "le": 55, "icv_min": 12, "icv_max": 18},</v>
+      </c>
+    </row>
+    <row r="70" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T70">
+        <v>56</v>
+      </c>
+      <c r="U70">
+        <v>57</v>
+      </c>
+      <c r="V70">
+        <v>11</v>
+      </c>
+      <c r="W70">
+        <v>18</v>
+      </c>
+      <c r="X70" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 56, "le": 57, "icv_min": 11, "icv_max": 18},</v>
+      </c>
+    </row>
+    <row r="71" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T71">
+        <v>58</v>
+      </c>
+      <c r="U71">
+        <v>59</v>
+      </c>
+      <c r="V71">
+        <v>10</v>
+      </c>
+      <c r="W71">
+        <v>18</v>
+      </c>
+      <c r="X71" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 58, "le": 59, "icv_min": 10, "icv_max": 18},</v>
+      </c>
+    </row>
+    <row r="72" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T72">
+        <v>60</v>
+      </c>
+      <c r="U72">
+        <v>61</v>
+      </c>
+      <c r="V72">
+        <v>9</v>
+      </c>
+      <c r="W72">
+        <v>18</v>
+      </c>
+      <c r="X72" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 60, "le": 61, "icv_min": 9, "icv_max": 18},</v>
+      </c>
+    </row>
+    <row r="73" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T73">
+        <v>62</v>
+      </c>
+      <c r="U73">
+        <v>65</v>
+      </c>
+      <c r="V73">
+        <v>14</v>
+      </c>
+      <c r="W73">
+        <v>15</v>
+      </c>
+      <c r="X73" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 62, "le": 65, "icv_min": 14, "icv_max": 15},</v>
+      </c>
+    </row>
+    <row r="74" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T74">
+        <v>66</v>
+      </c>
+      <c r="U74">
+        <v>69</v>
+      </c>
+      <c r="V74">
+        <v>13</v>
+      </c>
+      <c r="W74">
+        <v>15</v>
+      </c>
+      <c r="X74" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 66, "le": 69, "icv_min": 13, "icv_max": 15},</v>
+      </c>
+    </row>
+    <row r="75" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T75">
+        <v>70</v>
+      </c>
+      <c r="U75">
+        <v>73</v>
+      </c>
+      <c r="V75">
+        <v>12</v>
+      </c>
+      <c r="W75">
+        <v>15</v>
+      </c>
+      <c r="X75" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 70, "le": 73, "icv_min": 12, "icv_max": 15},</v>
+      </c>
+    </row>
+    <row r="76" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T76">
+        <v>74</v>
+      </c>
+      <c r="U76">
+        <v>77</v>
+      </c>
+      <c r="V76">
+        <v>11</v>
+      </c>
+      <c r="W76">
+        <v>15</v>
+      </c>
+      <c r="X76" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 74, "le": 77, "icv_min": 11, "icv_max": 15},</v>
+      </c>
+    </row>
+    <row r="77" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T77">
+        <v>78</v>
+      </c>
+      <c r="U77">
+        <v>81</v>
+      </c>
+      <c r="V77">
+        <v>10</v>
+      </c>
+      <c r="W77">
+        <v>15</v>
+      </c>
+      <c r="X77" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 78, "le": 81, "icv_min": 10, "icv_max": 15},</v>
+      </c>
+    </row>
+    <row r="78" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T78">
+        <v>82</v>
+      </c>
+      <c r="U78">
+        <v>85</v>
+      </c>
+      <c r="V78">
+        <v>9</v>
+      </c>
+      <c r="W78">
+        <v>15</v>
+      </c>
+      <c r="X78" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 82, "le": 85, "icv_min": 9, "icv_max": 15},</v>
+      </c>
+    </row>
+    <row r="79" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T79">
+        <v>86</v>
+      </c>
+      <c r="U79">
+        <v>89</v>
+      </c>
+      <c r="V79">
+        <v>8</v>
+      </c>
+      <c r="W79">
+        <v>15</v>
+      </c>
+      <c r="X79" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 86, "le": 89, "icv_min": 8, "icv_max": 15},</v>
+      </c>
+    </row>
+    <row r="80" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T80">
+        <v>90</v>
+      </c>
+      <c r="U80">
+        <v>93</v>
+      </c>
+      <c r="V80">
+        <v>7</v>
+      </c>
+      <c r="W80">
+        <v>15</v>
+      </c>
+      <c r="X80" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 90, "le": 93, "icv_min": 7, "icv_max": 15},</v>
+      </c>
+    </row>
+    <row r="81" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T81">
+        <v>94</v>
+      </c>
+      <c r="U81">
+        <v>97</v>
+      </c>
+      <c r="V81">
+        <v>6</v>
+      </c>
+      <c r="W81">
+        <v>15</v>
+      </c>
+      <c r="X81" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 94, "le": 97, "icv_min": 6, "icv_max": 15},</v>
+      </c>
+    </row>
+    <row r="82" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T82">
+        <v>98</v>
+      </c>
+      <c r="U82">
+        <v>105</v>
+      </c>
+      <c r="V82">
+        <v>11</v>
+      </c>
+      <c r="W82">
+        <v>12</v>
+      </c>
+      <c r="X82" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 98, "le": 105, "icv_min": 11, "icv_max": 12},</v>
+      </c>
+    </row>
+    <row r="83" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T83">
+        <v>106</v>
+      </c>
+      <c r="U83">
+        <v>113</v>
+      </c>
+      <c r="V83">
+        <v>10</v>
+      </c>
+      <c r="W83">
+        <v>12</v>
+      </c>
+      <c r="X83" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 106, "le": 113, "icv_min": 10, "icv_max": 12},</v>
+      </c>
+    </row>
+    <row r="84" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T84">
+        <v>114</v>
+      </c>
+      <c r="U84">
+        <v>121</v>
+      </c>
+      <c r="V84">
+        <v>9</v>
+      </c>
+      <c r="W84">
+        <v>12</v>
+      </c>
+      <c r="X84" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 114, "le": 121, "icv_min": 9, "icv_max": 12},</v>
+      </c>
+    </row>
+    <row r="85" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T85">
+        <v>122</v>
+      </c>
+      <c r="U85">
+        <v>129</v>
+      </c>
+      <c r="V85">
+        <v>8</v>
+      </c>
+      <c r="W85">
+        <v>12</v>
+      </c>
+      <c r="X85" t="str">
+        <f t="shared" si="6"/>
+        <v>{"ge": 122, "le": 129, "icv_min": 8, "icv_max": 12},</v>
+      </c>
+    </row>
+    <row r="86" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T86">
+        <v>130</v>
+      </c>
+      <c r="U86">
+        <v>137</v>
+      </c>
+      <c r="V86">
+        <v>7</v>
+      </c>
+      <c r="W86">
+        <v>12</v>
+      </c>
+      <c r="X86" t="str">
+        <f t="shared" ref="X86:X96" si="7">_xlfn.CONCAT("{""ge"": ",T86,", ""le"": ",U86,", ""icv_min"": ",V86,", ""icv_max"": ",W86,"},")</f>
+        <v>{"ge": 130, "le": 137, "icv_min": 7, "icv_max": 12},</v>
+      </c>
+    </row>
+    <row r="87" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T87">
+        <v>138</v>
+      </c>
+      <c r="U87">
+        <v>145</v>
+      </c>
+      <c r="V87">
+        <v>6</v>
+      </c>
+      <c r="W87">
+        <v>12</v>
+      </c>
+      <c r="X87" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 138, "le": 145, "icv_min": 6, "icv_max": 12},</v>
+      </c>
+    </row>
+    <row r="88" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T88">
+        <v>146</v>
+      </c>
+      <c r="U88">
+        <v>153</v>
+      </c>
+      <c r="V88">
+        <v>5</v>
+      </c>
+      <c r="W88">
+        <v>12</v>
+      </c>
+      <c r="X88" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 146, "le": 153, "icv_min": 5, "icv_max": 12},</v>
+      </c>
+    </row>
+    <row r="89" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T89">
+        <v>154</v>
+      </c>
+      <c r="U89">
+        <v>161</v>
+      </c>
+      <c r="V89">
+        <v>4</v>
+      </c>
+      <c r="W89">
+        <v>12</v>
+      </c>
+      <c r="X89" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 154, "le": 161, "icv_min": 4, "icv_max": 12},</v>
+      </c>
+    </row>
+    <row r="90" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T90">
+        <v>162</v>
+      </c>
+      <c r="U90">
+        <v>169</v>
+      </c>
+      <c r="V90">
+        <v>3</v>
+      </c>
+      <c r="W90">
+        <v>12</v>
+      </c>
+      <c r="X90" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 162, "le": 169, "icv_min": 3, "icv_max": 12},</v>
+      </c>
+    </row>
+    <row r="91" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T91">
+        <v>170</v>
+      </c>
+      <c r="U91">
+        <v>185</v>
+      </c>
+      <c r="V91">
+        <v>8</v>
+      </c>
+      <c r="W91">
+        <v>9</v>
+      </c>
+      <c r="X91" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 170, "le": 185, "icv_min": 8, "icv_max": 9},</v>
+      </c>
+    </row>
+    <row r="92" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T92">
+        <v>186</v>
+      </c>
+      <c r="U92">
+        <v>201</v>
+      </c>
+      <c r="V92">
+        <v>7</v>
+      </c>
+      <c r="W92">
+        <v>9</v>
+      </c>
+      <c r="X92" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 186, "le": 201, "icv_min": 7, "icv_max": 9},</v>
+      </c>
+    </row>
+    <row r="93" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T93">
+        <v>202</v>
+      </c>
+      <c r="U93">
+        <v>217</v>
+      </c>
+      <c r="V93">
+        <v>6</v>
+      </c>
+      <c r="W93">
+        <v>9</v>
+      </c>
+      <c r="X93" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 202, "le": 217, "icv_min": 6, "icv_max": 9},</v>
+      </c>
+    </row>
+    <row r="94" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T94">
+        <v>218</v>
+      </c>
+      <c r="U94">
+        <v>233</v>
+      </c>
+      <c r="V94">
+        <v>5</v>
+      </c>
+      <c r="W94">
+        <v>9</v>
+      </c>
+      <c r="X94" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 218, "le": 233, "icv_min": 5, "icv_max": 9},</v>
+      </c>
+    </row>
+    <row r="95" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T95">
+        <v>234</v>
+      </c>
+      <c r="U95">
+        <v>249</v>
+      </c>
+      <c r="V95">
+        <v>4</v>
+      </c>
+      <c r="W95">
+        <v>9</v>
+      </c>
+      <c r="X95" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 234, "le": 249, "icv_min": 4, "icv_max": 9},</v>
+      </c>
+    </row>
+    <row r="96" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T96">
+        <v>250</v>
+      </c>
+      <c r="U96">
+        <v>255</v>
+      </c>
+      <c r="V96">
+        <v>3</v>
+      </c>
+      <c r="W96">
+        <v>9</v>
+      </c>
+      <c r="X96" t="str">
+        <f t="shared" si="7"/>
+        <v>{"ge": 250, "le": 255, "icv_min": 3, "icv_max": 9},</v>
       </c>
     </row>
   </sheetData>
@@ -1725,7 +3790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E66D53-D2EC-4F50-B03A-ADFEA94349BE}">
   <dimension ref="A2:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -3743,7 +5808,7 @@
         <v>941234</v>
       </c>
       <c r="D98" s="8">
-        <f t="shared" ref="D98:D129" si="8">C98/B98</f>
+        <f t="shared" ref="D98:D102" si="8">C98/B98</f>
         <v>188246.8</v>
       </c>
     </row>

</xml_diff>